<commit_message>
Update Sorter Inspection Validation Indy.xlsx
</commit_message>
<xml_diff>
--- a/data/Sorter Inspection Validation Indy.xlsx
+++ b/data/Sorter Inspection Validation Indy.xlsx
@@ -659,12 +659,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Strand 4</t>
+          <t>Strand 1</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>1:54:01</t>
+          <t>1:16:39</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -709,12 +709,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Strand 1</t>
+          <t>Strand 4</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>1:16:39</t>
+          <t>1:54:01</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -834,12 +834,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Strand 4</t>
+          <t>Strand 5</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>1:06:08</t>
+          <t>1:39:45</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -859,12 +859,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Strand 5</t>
+          <t>Strand 4</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>1:39:45</t>
+          <t>1:06:08</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -884,12 +884,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Strand 8</t>
+          <t>Strand 2</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>1:34:13</t>
+          <t>1:40:37</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -909,17 +909,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Strand 2</t>
+          <t>Strand 1</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>1:40:37</t>
+          <t>1:30:27</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E18" s="3" t="inlineStr">
@@ -934,17 +934,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Strand 1</t>
+          <t>Strand 8</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>1:30:27</t>
+          <t>1:34:13</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E19" s="3" t="inlineStr">
@@ -1009,22 +1009,22 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Strand 3</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>0:11:24</t>
+          <t>Strand 5</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="inlineStr">
+        <is>
+          <t>1:50:47</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="E22" s="2" t="inlineStr">
-        <is>
-          <t>Fail</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E22" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
@@ -1034,22 +1034,22 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Strand 5</t>
-        </is>
-      </c>
-      <c r="C23" s="3" t="inlineStr">
-        <is>
-          <t>1:50:47</t>
+          <t>Strand 3</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="inlineStr">
+        <is>
+          <t>0:11:24</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E23" s="3" t="inlineStr">
-        <is>
-          <t>Pass</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>Fail</t>
         </is>
       </c>
     </row>
@@ -1184,12 +1184,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Strand 8</t>
+          <t>Strand 1</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
         <is>
-          <t>1:42:41</t>
+          <t>1:29:40</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1209,12 +1209,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Strand 1</t>
+          <t>Strand 8</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
         <is>
-          <t>1:29:40</t>
+          <t>1:42:41</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1259,12 +1259,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Strand 4</t>
-        </is>
-      </c>
-      <c r="C32" s="2" t="inlineStr">
-        <is>
-          <t>0:01:46</t>
+          <t>Strand 5</t>
+        </is>
+      </c>
+      <c r="C32" s="3" t="inlineStr">
+        <is>
+          <t>1:40:49</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1272,9 +1272,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E32" s="2" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="E32" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
@@ -1284,12 +1284,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Strand 5</t>
-        </is>
-      </c>
-      <c r="C33" s="3" t="inlineStr">
-        <is>
-          <t>1:40:49</t>
+          <t>Strand 4</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="inlineStr">
+        <is>
+          <t>0:01:46</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1297,9 +1297,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E33" s="3" t="inlineStr">
-        <is>
-          <t>Pass</t>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>Fail</t>
         </is>
       </c>
     </row>
@@ -1434,17 +1434,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Strand 8</t>
+          <t>Strand 1</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
         <is>
-          <t>1:29:25</t>
+          <t>1:36:51</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E39" s="3" t="inlineStr">
@@ -1459,17 +1459,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Strand 1</t>
+          <t>Strand 8</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
         <is>
-          <t>1:36:51</t>
+          <t>1:29:25</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E40" s="3" t="inlineStr">
@@ -1584,17 +1584,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Strand 8</t>
+          <t>Strand 1</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
         <is>
-          <t>1:50:48</t>
+          <t>1:35:26</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E45" s="3" t="inlineStr">
@@ -1609,17 +1609,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Strand 1</t>
+          <t>Strand 8</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>1:35:26</t>
+          <t>1:50:48</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E46" s="3" t="inlineStr">
@@ -1634,17 +1634,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Strand 4</t>
+          <t>Strand 3</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>1:24:11</t>
+          <t>2:00:05</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E47" s="3" t="inlineStr">
@@ -1659,17 +1659,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Strand 3</t>
+          <t>Strand 4</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
         <is>
-          <t>2:00:05</t>
+          <t>1:24:11</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E48" s="3" t="inlineStr">
@@ -1684,12 +1684,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Strand 6</t>
+          <t>Strand 5</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
         <is>
-          <t>1:08:23</t>
+          <t>1:41:15</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1709,12 +1709,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Strand 5</t>
+          <t>Strand 6</t>
         </is>
       </c>
       <c r="C50" s="3" t="inlineStr">
         <is>
-          <t>1:41:15</t>
+          <t>1:08:23</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1784,12 +1784,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Strand 8</t>
+          <t>Strand 1</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr">
         <is>
-          <t>1:18:57</t>
+          <t>1:45:58</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1809,12 +1809,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Strand 1</t>
+          <t>Strand 8</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr">
         <is>
-          <t>1:45:58</t>
+          <t>1:18:57</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1934,12 +1934,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Strand 4</t>
+          <t>Strand 8</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr">
         <is>
-          <t>1:02:01</t>
+          <t>1:54:10</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1959,12 +1959,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Strand 8</t>
+          <t>Strand 4</t>
         </is>
       </c>
       <c r="C60" s="3" t="inlineStr">
         <is>
-          <t>1:54:10</t>
+          <t>1:02:01</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2084,22 +2084,22 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Strand 3</t>
-        </is>
-      </c>
-      <c r="C65" s="2" t="inlineStr">
-        <is>
-          <t>0:44:40</t>
+          <t>Strand 2</t>
+        </is>
+      </c>
+      <c r="C65" s="3" t="inlineStr">
+        <is>
+          <t>2:47:24</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="E65" s="2" t="inlineStr">
-        <is>
-          <t>Fail</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E65" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
@@ -2109,12 +2109,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Strand 8</t>
-        </is>
-      </c>
-      <c r="C66" s="3" t="inlineStr">
-        <is>
-          <t>1:30:11</t>
+          <t>Strand 1</t>
+        </is>
+      </c>
+      <c r="C66" s="2" t="inlineStr">
+        <is>
+          <t>0:27:40</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2122,9 +2122,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E66" s="3" t="inlineStr">
-        <is>
-          <t>Pass</t>
+      <c r="E66" s="2" t="inlineStr">
+        <is>
+          <t>Fail</t>
         </is>
       </c>
     </row>
@@ -2134,17 +2134,17 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Strand 2</t>
+          <t>Strand 5</t>
         </is>
       </c>
       <c r="C67" s="3" t="inlineStr">
         <is>
-          <t>2:47:24</t>
+          <t>1:26:12</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E67" s="3" t="inlineStr">
@@ -2159,17 +2159,17 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Strand 1</t>
+          <t>Strand 3</t>
         </is>
       </c>
       <c r="C68" s="2" t="inlineStr">
         <is>
-          <t>0:27:40</t>
+          <t>0:44:40</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E68" s="2" t="inlineStr">
@@ -2184,17 +2184,17 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Strand 5</t>
+          <t>Strand 8</t>
         </is>
       </c>
       <c r="C69" s="3" t="inlineStr">
         <is>
-          <t>1:26:12</t>
+          <t>1:30:11</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E69" s="3" t="inlineStr">
@@ -2234,12 +2234,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Strand 4</t>
-        </is>
-      </c>
-      <c r="C71" s="3" t="inlineStr">
-        <is>
-          <t>1:40:32</t>
+          <t>Strand 5</t>
+        </is>
+      </c>
+      <c r="C71" s="2" t="inlineStr">
+        <is>
+          <t>0:41:13</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2247,9 +2247,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E71" s="3" t="inlineStr">
-        <is>
-          <t>Pass</t>
+      <c r="E71" s="2" t="inlineStr">
+        <is>
+          <t>Fail</t>
         </is>
       </c>
     </row>
@@ -2309,12 +2309,12 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Strand 5</t>
-        </is>
-      </c>
-      <c r="C74" s="2" t="inlineStr">
-        <is>
-          <t>0:41:13</t>
+          <t>Strand 4</t>
+        </is>
+      </c>
+      <c r="C74" s="3" t="inlineStr">
+        <is>
+          <t>1:40:32</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2322,9 +2322,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E74" s="2" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="E74" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
@@ -2434,12 +2434,12 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Strand 4</t>
-        </is>
-      </c>
-      <c r="C79" s="3" t="inlineStr">
-        <is>
-          <t>1:34:57</t>
+          <t>Strand 2</t>
+        </is>
+      </c>
+      <c r="C79" s="2" t="inlineStr">
+        <is>
+          <t>0:17:48</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2447,9 +2447,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E79" s="3" t="inlineStr">
-        <is>
-          <t>Pass</t>
+      <c r="E79" s="2" t="inlineStr">
+        <is>
+          <t>Fail</t>
         </is>
       </c>
     </row>
@@ -2459,12 +2459,12 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Strand 3</t>
+          <t>Strand 1</t>
         </is>
       </c>
       <c r="C80" s="3" t="inlineStr">
         <is>
-          <t>1:51:42</t>
+          <t>3:35:22</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2484,12 +2484,12 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Strand 8</t>
-        </is>
-      </c>
-      <c r="C81" s="2" t="inlineStr">
-        <is>
-          <t>0:38:37</t>
+          <t>Strand 5</t>
+        </is>
+      </c>
+      <c r="C81" s="3" t="inlineStr">
+        <is>
+          <t>2:59:00</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2497,9 +2497,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E81" s="2" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="E81" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
@@ -2509,12 +2509,12 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Strand 2</t>
-        </is>
-      </c>
-      <c r="C82" s="2" t="inlineStr">
-        <is>
-          <t>0:17:48</t>
+          <t>Strand 3</t>
+        </is>
+      </c>
+      <c r="C82" s="3" t="inlineStr">
+        <is>
+          <t>1:51:42</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2522,9 +2522,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E82" s="2" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="E82" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
@@ -2534,12 +2534,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Strand 1</t>
-        </is>
-      </c>
-      <c r="C83" s="3" t="inlineStr">
-        <is>
-          <t>3:35:22</t>
+          <t>Strand 8</t>
+        </is>
+      </c>
+      <c r="C83" s="2" t="inlineStr">
+        <is>
+          <t>0:38:37</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2547,9 +2547,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E83" s="3" t="inlineStr">
-        <is>
-          <t>Pass</t>
+      <c r="E83" s="2" t="inlineStr">
+        <is>
+          <t>Fail</t>
         </is>
       </c>
     </row>
@@ -2559,12 +2559,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Strand 5</t>
+          <t>Strand 4</t>
         </is>
       </c>
       <c r="C84" s="3" t="inlineStr">
         <is>
-          <t>2:59:00</t>
+          <t>1:34:57</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2659,12 +2659,12 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Strand 4</t>
-        </is>
-      </c>
-      <c r="C88" s="2" t="inlineStr">
-        <is>
-          <t>0:24:49</t>
+          <t>Strand 1</t>
+        </is>
+      </c>
+      <c r="C88" s="3" t="inlineStr">
+        <is>
+          <t>2:54:06</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2672,9 +2672,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E88" s="2" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="E88" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
@@ -2684,12 +2684,12 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Strand 3</t>
+          <t>Strand 5</t>
         </is>
       </c>
       <c r="C89" s="2" t="inlineStr">
         <is>
-          <t>0:36:19</t>
+          <t>0:00:03</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2709,12 +2709,12 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Strand 1</t>
-        </is>
-      </c>
-      <c r="C90" s="3" t="inlineStr">
-        <is>
-          <t>2:54:06</t>
+          <t>Strand 3</t>
+        </is>
+      </c>
+      <c r="C90" s="2" t="inlineStr">
+        <is>
+          <t>0:36:19</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -2722,9 +2722,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E90" s="3" t="inlineStr">
-        <is>
-          <t>Pass</t>
+      <c r="E90" s="2" t="inlineStr">
+        <is>
+          <t>Fail</t>
         </is>
       </c>
     </row>
@@ -2734,12 +2734,12 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Strand 5</t>
+          <t>Strand 4</t>
         </is>
       </c>
       <c r="C91" s="2" t="inlineStr">
         <is>
-          <t>0:00:03</t>
+          <t>0:24:49</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2834,12 +2834,12 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Strand 6</t>
-        </is>
-      </c>
-      <c r="C95" s="2" t="inlineStr">
-        <is>
-          <t>0:01:38</t>
+          <t>Strand 2</t>
+        </is>
+      </c>
+      <c r="C95" s="3" t="inlineStr">
+        <is>
+          <t>1:16:58</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2847,9 +2847,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E95" s="2" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="E95" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
@@ -2859,12 +2859,12 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Strand 2</t>
-        </is>
-      </c>
-      <c r="C96" s="3" t="inlineStr">
-        <is>
-          <t>1:16:58</t>
+          <t>Strand 5</t>
+        </is>
+      </c>
+      <c r="C96" s="2" t="inlineStr">
+        <is>
+          <t>0:08:44</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2872,9 +2872,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E96" s="3" t="inlineStr">
-        <is>
-          <t>Pass</t>
+      <c r="E96" s="2" t="inlineStr">
+        <is>
+          <t>Fail</t>
         </is>
       </c>
     </row>
@@ -2884,12 +2884,12 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Strand 5</t>
+          <t>Strand 6</t>
         </is>
       </c>
       <c r="C97" s="2" t="inlineStr">
         <is>
-          <t>0:08:44</t>
+          <t>0:01:38</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2934,12 +2934,12 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Strand 3</t>
+          <t>Strand 5</t>
         </is>
       </c>
       <c r="C99" s="3" t="inlineStr">
         <is>
-          <t>1:26:43</t>
+          <t>1:35:44</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -2959,12 +2959,12 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Strand 5</t>
+          <t>Strand 3</t>
         </is>
       </c>
       <c r="C100" s="3" t="inlineStr">
         <is>
-          <t>1:35:44</t>
+          <t>1:26:43</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -2984,12 +2984,12 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Strand 4</t>
-        </is>
-      </c>
-      <c r="C101" s="3" t="inlineStr">
-        <is>
-          <t>1:31:53</t>
+          <t>Strand 6</t>
+        </is>
+      </c>
+      <c r="C101" s="2" t="inlineStr">
+        <is>
+          <t>0:28:16</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -2997,9 +2997,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E101" s="3" t="inlineStr">
-        <is>
-          <t>Pass</t>
+      <c r="E101" s="2" t="inlineStr">
+        <is>
+          <t>Fail</t>
         </is>
       </c>
     </row>
@@ -3009,12 +3009,12 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Strand 6</t>
-        </is>
-      </c>
-      <c r="C102" s="2" t="inlineStr">
-        <is>
-          <t>0:28:16</t>
+          <t>Strand 4</t>
+        </is>
+      </c>
+      <c r="C102" s="3" t="inlineStr">
+        <is>
+          <t>1:31:53</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3022,9 +3022,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E102" s="2" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="E102" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
@@ -3109,12 +3109,12 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Strand 3</t>
-        </is>
-      </c>
-      <c r="C106" s="3" t="inlineStr">
-        <is>
-          <t>1:28:54</t>
+          <t>Strand 2</t>
+        </is>
+      </c>
+      <c r="C106" s="2" t="inlineStr">
+        <is>
+          <t>0:18:14</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3122,9 +3122,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E106" s="3" t="inlineStr">
-        <is>
-          <t>Pass</t>
+      <c r="E106" s="2" t="inlineStr">
+        <is>
+          <t>Fail</t>
         </is>
       </c>
     </row>
@@ -3134,12 +3134,12 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Strand 2</t>
-        </is>
-      </c>
-      <c r="C107" s="2" t="inlineStr">
-        <is>
-          <t>0:18:14</t>
+          <t>Strand 3</t>
+        </is>
+      </c>
+      <c r="C107" s="3" t="inlineStr">
+        <is>
+          <t>1:28:54</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3147,9 +3147,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E107" s="2" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="E107" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
@@ -3159,12 +3159,12 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Strand 3</t>
-        </is>
-      </c>
-      <c r="C108" s="2" t="inlineStr">
-        <is>
-          <t>0:23:04</t>
+          <t>Strand 5</t>
+        </is>
+      </c>
+      <c r="C108" s="3" t="inlineStr">
+        <is>
+          <t>3:08:31</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3172,9 +3172,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E108" s="2" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="E108" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
@@ -3184,12 +3184,12 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Strand 8</t>
-        </is>
-      </c>
-      <c r="C109" s="3" t="inlineStr">
-        <is>
-          <t>1:24:32</t>
+          <t>Strand 3</t>
+        </is>
+      </c>
+      <c r="C109" s="2" t="inlineStr">
+        <is>
+          <t>0:23:04</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3197,9 +3197,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E109" s="3" t="inlineStr">
-        <is>
-          <t>Pass</t>
+      <c r="E109" s="2" t="inlineStr">
+        <is>
+          <t>Fail</t>
         </is>
       </c>
     </row>
@@ -3209,12 +3209,12 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Strand 5</t>
+          <t>Strand 8</t>
         </is>
       </c>
       <c r="C110" s="3" t="inlineStr">
         <is>
-          <t>3:08:31</t>
+          <t>1:24:32</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3309,12 +3309,12 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Strand 8</t>
+          <t>Strand 1</t>
         </is>
       </c>
       <c r="C114" s="3" t="inlineStr">
         <is>
-          <t>1:36:15</t>
+          <t>1:07:48</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3334,12 +3334,12 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Strand 1</t>
+          <t>Strand 8</t>
         </is>
       </c>
       <c r="C115" s="3" t="inlineStr">
         <is>
-          <t>1:07:48</t>
+          <t>1:36:15</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -3384,12 +3384,12 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Strand 6</t>
+          <t>Strand 5</t>
         </is>
       </c>
       <c r="C117" s="3" t="inlineStr">
         <is>
-          <t>1:12:47</t>
+          <t>1:18:54</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3409,12 +3409,12 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Strand 5</t>
+          <t>Strand 6</t>
         </is>
       </c>
       <c r="C118" s="3" t="inlineStr">
         <is>
-          <t>1:18:54</t>
+          <t>1:12:47</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3459,17 +3459,17 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Strand 4</t>
+          <t>Strand 8</t>
         </is>
       </c>
       <c r="C120" s="2" t="inlineStr">
         <is>
-          <t>0:12:06</t>
+          <t>0:13:28</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E120" s="2" t="inlineStr">
@@ -3484,17 +3484,17 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Strand 8</t>
+          <t>Strand 4</t>
         </is>
       </c>
       <c r="C121" s="2" t="inlineStr">
         <is>
-          <t>0:13:28</t>
+          <t>0:12:06</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E121" s="2" t="inlineStr">
@@ -3534,12 +3534,12 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Strand 4</t>
-        </is>
-      </c>
-      <c r="C123" s="3" t="inlineStr">
-        <is>
-          <t>1:31:47</t>
+          <t>Strand 5</t>
+        </is>
+      </c>
+      <c r="C123" s="2" t="inlineStr">
+        <is>
+          <t>0:45:45</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -3547,9 +3547,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E123" s="3" t="inlineStr">
-        <is>
-          <t>Pass</t>
+      <c r="E123" s="2" t="inlineStr">
+        <is>
+          <t>Fail</t>
         </is>
       </c>
     </row>
@@ -3609,12 +3609,12 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Strand 5</t>
-        </is>
-      </c>
-      <c r="C126" s="2" t="inlineStr">
-        <is>
-          <t>0:45:45</t>
+          <t>Strand 4</t>
+        </is>
+      </c>
+      <c r="C126" s="3" t="inlineStr">
+        <is>
+          <t>1:31:47</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -3622,9 +3622,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E126" s="2" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="E126" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
@@ -3684,17 +3684,17 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Strand 4</t>
+          <t>Strand 5</t>
         </is>
       </c>
       <c r="C129" s="3" t="inlineStr">
         <is>
-          <t>1:44:20</t>
+          <t>1:01:10</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E129" s="3" t="inlineStr">
@@ -3709,12 +3709,12 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Strand 3</t>
-        </is>
-      </c>
-      <c r="C130" s="3" t="inlineStr">
-        <is>
-          <t>2:10:10</t>
+          <t>Strand 6</t>
+        </is>
+      </c>
+      <c r="C130" s="2" t="inlineStr">
+        <is>
+          <t>0:26:24</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -3722,9 +3722,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E130" s="3" t="inlineStr">
-        <is>
-          <t>Pass</t>
+      <c r="E130" s="2" t="inlineStr">
+        <is>
+          <t>Fail</t>
         </is>
       </c>
     </row>
@@ -3734,12 +3734,12 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Strand 6</t>
-        </is>
-      </c>
-      <c r="C131" s="2" t="inlineStr">
-        <is>
-          <t>0:26:24</t>
+          <t>Strand 3</t>
+        </is>
+      </c>
+      <c r="C131" s="3" t="inlineStr">
+        <is>
+          <t>2:10:10</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -3747,9 +3747,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E131" s="2" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="E131" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
@@ -3784,17 +3784,17 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Strand 5</t>
+          <t>Strand 4</t>
         </is>
       </c>
       <c r="C133" s="3" t="inlineStr">
         <is>
-          <t>1:01:10</t>
+          <t>1:44:20</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E133" s="3" t="inlineStr">
@@ -3884,12 +3884,12 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Strand 3</t>
+          <t>Strand 5</t>
         </is>
       </c>
       <c r="C137" s="2" t="inlineStr">
         <is>
-          <t>0:09:56</t>
+          <t>0:13:13</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -3934,12 +3934,12 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Strand 5</t>
+          <t>Strand 3</t>
         </is>
       </c>
       <c r="C139" s="2" t="inlineStr">
         <is>
-          <t>0:13:13</t>
+          <t>0:09:56</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -4034,12 +4034,12 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Strand 8</t>
-        </is>
-      </c>
-      <c r="C143" s="2" t="inlineStr">
-        <is>
-          <t>0:45:51</t>
+          <t>Strand 1</t>
+        </is>
+      </c>
+      <c r="C143" s="4" t="inlineStr">
+        <is>
+          <t>0:51:47</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -4059,12 +4059,12 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Strand 1</t>
-        </is>
-      </c>
-      <c r="C144" s="4" t="inlineStr">
-        <is>
-          <t>0:51:47</t>
+          <t>Strand 8</t>
+        </is>
+      </c>
+      <c r="C144" s="2" t="inlineStr">
+        <is>
+          <t>0:45:51</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -4134,17 +4134,17 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Strand 8</t>
+          <t>Strand 1</t>
         </is>
       </c>
       <c r="C147" s="3" t="inlineStr">
         <is>
-          <t>5:06:45</t>
+          <t>2:24:32</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E147" s="3" t="inlineStr">
@@ -4159,12 +4159,12 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Strand 1</t>
+          <t>Strand 5</t>
         </is>
       </c>
       <c r="C148" s="3" t="inlineStr">
         <is>
-          <t>2:24:32</t>
+          <t>1:09:01</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -4184,17 +4184,17 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Strand 5</t>
+          <t>Strand 8</t>
         </is>
       </c>
       <c r="C149" s="3" t="inlineStr">
         <is>
-          <t>1:09:01</t>
+          <t>5:06:45</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E149" s="3" t="inlineStr">
@@ -4209,22 +4209,22 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Strand 4</t>
-        </is>
-      </c>
-      <c r="C150" s="3" t="inlineStr">
-        <is>
-          <t>1:42:25</t>
+          <t>Strand 1</t>
+        </is>
+      </c>
+      <c r="C150" s="2" t="inlineStr">
+        <is>
+          <t>0:10:35</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E150" s="3" t="inlineStr">
-        <is>
-          <t>Pass</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E150" s="2" t="inlineStr">
+        <is>
+          <t>Fail</t>
         </is>
       </c>
     </row>
@@ -4259,22 +4259,22 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Strand 1</t>
-        </is>
-      </c>
-      <c r="C152" s="2" t="inlineStr">
-        <is>
-          <t>0:10:35</t>
+          <t>Strand 4</t>
+        </is>
+      </c>
+      <c r="C152" s="3" t="inlineStr">
+        <is>
+          <t>1:42:25</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="E152" s="2" t="inlineStr">
-        <is>
-          <t>Fail</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E152" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
@@ -4284,12 +4284,12 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Strand 4</t>
-        </is>
-      </c>
-      <c r="C153" s="2" t="inlineStr">
-        <is>
-          <t>0:16:23</t>
+          <t>Strand 6</t>
+        </is>
+      </c>
+      <c r="C153" s="3" t="inlineStr">
+        <is>
+          <t>1:39:42</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -4297,9 +4297,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E153" s="2" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="E153" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
@@ -4309,12 +4309,12 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Strand 6</t>
+          <t>Strand 8</t>
         </is>
       </c>
       <c r="C154" s="3" t="inlineStr">
         <is>
-          <t>1:39:42</t>
+          <t>1:12:37</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -4334,12 +4334,12 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Strand 8</t>
-        </is>
-      </c>
-      <c r="C155" s="3" t="inlineStr">
-        <is>
-          <t>1:12:37</t>
+          <t>Strand 4</t>
+        </is>
+      </c>
+      <c r="C155" s="2" t="inlineStr">
+        <is>
+          <t>0:16:23</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -4347,9 +4347,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E155" s="3" t="inlineStr">
-        <is>
-          <t>Pass</t>
+      <c r="E155" s="2" t="inlineStr">
+        <is>
+          <t>Fail</t>
         </is>
       </c>
     </row>
@@ -4409,22 +4409,22 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Strand 6</t>
-        </is>
-      </c>
-      <c r="C158" s="3" t="inlineStr">
-        <is>
-          <t>1:40:46</t>
+          <t>Strand 2</t>
+        </is>
+      </c>
+      <c r="C158" s="2" t="inlineStr">
+        <is>
+          <t>0:42:58</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="E158" s="3" t="inlineStr">
-        <is>
-          <t>Pass</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E158" s="2" t="inlineStr">
+        <is>
+          <t>Fail</t>
         </is>
       </c>
     </row>
@@ -4434,12 +4434,12 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Strand 2</t>
+          <t>Strand 1</t>
         </is>
       </c>
       <c r="C159" s="2" t="inlineStr">
         <is>
-          <t>0:42:58</t>
+          <t>0:41:47</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -4459,22 +4459,22 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Strand 1</t>
-        </is>
-      </c>
-      <c r="C160" s="2" t="inlineStr">
-        <is>
-          <t>0:41:47</t>
+          <t>Strand 6</t>
+        </is>
+      </c>
+      <c r="C160" s="3" t="inlineStr">
+        <is>
+          <t>1:40:46</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E160" s="2" t="inlineStr">
-        <is>
-          <t>Fail</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E160" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
@@ -4534,12 +4534,12 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Strand 4</t>
-        </is>
-      </c>
-      <c r="C163" s="4" t="inlineStr">
-        <is>
-          <t>0:56:50</t>
+          <t>Strand 3</t>
+        </is>
+      </c>
+      <c r="C163" s="3" t="inlineStr">
+        <is>
+          <t>1:12:46</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
@@ -4547,9 +4547,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E163" s="2" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="E163" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
@@ -4559,12 +4559,12 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Strand 3</t>
-        </is>
-      </c>
-      <c r="C164" s="3" t="inlineStr">
-        <is>
-          <t>1:12:46</t>
+          <t>Strand 4</t>
+        </is>
+      </c>
+      <c r="C164" s="4" t="inlineStr">
+        <is>
+          <t>0:56:50</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
@@ -4572,9 +4572,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E164" s="3" t="inlineStr">
-        <is>
-          <t>Pass</t>
+      <c r="E164" s="2" t="inlineStr">
+        <is>
+          <t>Fail</t>
         </is>
       </c>
     </row>
@@ -4584,12 +4584,12 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Strand 8</t>
-        </is>
-      </c>
-      <c r="C165" s="2" t="inlineStr">
-        <is>
-          <t>0:41:34</t>
+          <t>Strand 1</t>
+        </is>
+      </c>
+      <c r="C165" s="4" t="inlineStr">
+        <is>
+          <t>0:56:24</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
@@ -4609,12 +4609,12 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Strand 1</t>
-        </is>
-      </c>
-      <c r="C166" s="4" t="inlineStr">
-        <is>
-          <t>0:56:24</t>
+          <t>Strand 8</t>
+        </is>
+      </c>
+      <c r="C166" s="2" t="inlineStr">
+        <is>
+          <t>0:41:34</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
@@ -4634,12 +4634,12 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Strand 6</t>
-        </is>
-      </c>
-      <c r="C167" s="2" t="inlineStr">
-        <is>
-          <t>0:49:17</t>
+          <t>Strand 2</t>
+        </is>
+      </c>
+      <c r="C167" s="3" t="inlineStr">
+        <is>
+          <t>1:06:15</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
@@ -4647,9 +4647,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E167" s="2" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="E167" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
@@ -4659,12 +4659,12 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Strand 2</t>
-        </is>
-      </c>
-      <c r="C168" s="3" t="inlineStr">
-        <is>
-          <t>1:06:15</t>
+          <t>Strand 6</t>
+        </is>
+      </c>
+      <c r="C168" s="2" t="inlineStr">
+        <is>
+          <t>0:49:17</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
@@ -4672,9 +4672,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="E168" s="3" t="inlineStr">
-        <is>
-          <t>Pass</t>
+      <c r="E168" s="2" t="inlineStr">
+        <is>
+          <t>Fail</t>
         </is>
       </c>
     </row>
@@ -4725,7 +4725,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>01-05-25 to 01-11-25</t>
+          <t>01-04-25 to 01-10-25</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -4742,29 +4742,29 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>01-12-25 to 01-18-25</t>
+          <t>01-11-25 to 01-17-25</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Strand 1, Strand 2, Strand 3, Strand 4, Strand 5, Strand 6, Strand 7, Strand 8</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>Pass</t>
+          <t>Strand 1, Strand 2, Strand 3, Strand 4, Strand 6, Strand 7, Strand 8</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Fail</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>01-19-25 to 01-25-25</t>
+          <t>01-18-25 to 01-24-25</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Strand 1, Strand 2, Strand 3, Strand 4, Strand 5, Strand 6, Strand 8</t>
+          <t>Strand 1, Strand 2, Strand 3, Strand 4, Strand 5, Strand 8</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
@@ -4776,7 +4776,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>01-26-25 to 02-01-25</t>
+          <t>01-25-25 to 01-31-25</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -4793,7 +4793,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>02-02-25 to 02-08-25</t>
+          <t>02-01-25 to 02-07-25</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -4810,24 +4810,24 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>02-09-25 to 02-15-25</t>
+          <t>02-08-25 to 02-14-25</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Strand 1, Strand 2, Strand 3, Strand 4, Strand 5, Strand 6, Strand 7, Strand 8</t>
-        </is>
-      </c>
-      <c r="C7" s="3" t="inlineStr">
-        <is>
-          <t>Pass</t>
+          <t>Strand 1, Strand 2, Strand 3, Strand 4, Strand 7, Strand 8</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>Fail</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>02-16-25 to 02-22-25</t>
+          <t>02-15-25 to 02-21-25</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -4844,12 +4844,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>02-23-25 to 03-01-25</t>
+          <t>02-22-25 to 02-28-25</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Strand 2, Strand 4, Strand 5, Strand 6, Strand 8</t>
+          <t>Strand 2, Strand 4, Strand 5, Strand 8</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr">
@@ -4861,12 +4861,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>03-02-25 to 03-08-25</t>
+          <t>03-01-25 to 03-07-25</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Strand 1, Strand 2, Strand 3, Strand 5, Strand 7, Strand 8</t>
+          <t>Strand 1, Strand 2, Strand 3, Strand 5, Strand 6, Strand 7, Strand 8</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
@@ -4878,7 +4878,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>03-09-25 to 03-15-25</t>
+          <t>03-08-25 to 03-14-25</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -4895,7 +4895,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>03-16-25 to 03-22-25</t>
+          <t>03-15-25 to 03-21-25</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -4912,7 +4912,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>03-23-25 to 03-29-25</t>
+          <t>03-22-25 to 03-28-25</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -4929,7 +4929,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03-30-25 to 04-05-25</t>
+          <t>03-29-25 to 04-04-25</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -4946,12 +4946,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>04-06-25 to 04-12-25</t>
+          <t>04-05-25 to 04-11-25</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Strand 2, Strand 3, Strand 4, Strand 5, Strand 7, Strand 8</t>
+          <t>Strand 2, Strand 3, Strand 4, Strand 5, Strand 8</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr">
@@ -4963,7 +4963,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>04-13-25 to 04-19-25</t>
+          <t>04-12-25 to 04-18-25</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -4980,7 +4980,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>04-20-25 to 04-26-25</t>
+          <t>04-19-25 to 04-25-25</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -4997,7 +4997,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>04-27-25 to 05-03-25</t>
+          <t>04-26-25 to 05-02-25</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -5014,12 +5014,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>05-04-25 to 05-10-25</t>
+          <t>05-03-25 to 05-09-25</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Strand 1, Strand 3, Strand 5, Strand 6, Strand 8</t>
+          <t>Strand 1, Strand 3, Strand 5, Strand 6</t>
         </is>
       </c>
       <c r="C19" s="2" t="inlineStr">
@@ -5031,7 +5031,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>05-11-25 to 05-17-25</t>
+          <t>05-10-25 to 05-16-25</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -5048,29 +5048,29 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>05-18-25 to 05-24-25</t>
+          <t>05-17-25 to 05-23-25</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Strand 1, Strand 2, Strand 3, Strand 4, Strand 6, Strand 7, Strand 8</t>
-        </is>
-      </c>
-      <c r="C21" s="2" t="inlineStr">
-        <is>
-          <t>Fail</t>
+          <t>Strand 1, Strand 2, Strand 3, Strand 4, Strand 5, Strand 6, Strand 7, Strand 8</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>05-25-25 to 05-31-25</t>
+          <t>05-24-25 to 05-30-25</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Strand 2, Strand 6</t>
+          <t>Strand 1, Strand 2, Strand 6, Strand 8</t>
         </is>
       </c>
       <c r="C22" s="2" t="inlineStr">

</xml_diff>